<commit_message>
Work Work Work aaaarrrgggghhhh
</commit_message>
<xml_diff>
--- a/BTEC/BTEC.xlsx
+++ b/BTEC/BTEC.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\College\BTEC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="11040" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="11040" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Unit</t>
   </si>
@@ -33,28 +38,22 @@
     <t>2/2</t>
   </si>
   <si>
-    <t>0/1</t>
-  </si>
-  <si>
-    <t>0/?</t>
-  </si>
-  <si>
     <t>0/2</t>
   </si>
   <si>
-    <t>0.4/1</t>
-  </si>
-  <si>
     <t>1.1/2</t>
   </si>
   <si>
-    <t>1/1</t>
+    <t>1/2</t>
+  </si>
+  <si>
+    <t>0.4/2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -93,6 +92,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -421,15 +428,15 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -445,7 +452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -453,7 +460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -461,109 +468,80 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
-        <v>40</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>42</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>